<commit_message>
add reaction_9, which has no dependencies; remove data from test_dependencies.xlsx left over from coping its initial version from test_dynamic_expressions.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="1440" windowWidth="27380" windowHeight="9320" tabRatio="993" firstSheet="3" activeTab="10"/>
-    <workbookView xWindow="2360" yWindow="10860" windowWidth="31800" windowHeight="9920" tabRatio="500" firstSheet="9" activeTab="17"/>
+    <workbookView xWindow="-30900" yWindow="2100" windowWidth="29020" windowHeight="17400" tabRatio="993" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="820" yWindow="4560" windowWidth="31800" windowHeight="14380" tabRatio="500" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <definedName name="density_comp">'!!Parameters'!$D$15</definedName>
     <definedName name="NA">'!!Parameters'!$D$14</definedName>
     <definedName name="vol_comp">'!!Compartments'!$I$4</definedName>
-    <definedName name="volume_comp">'!!Functions'!$J$11</definedName>
+    <definedName name="volume_comp">'!!Functions'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="333">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -329,12 +329,6 @@
     <t>!Initial density</t>
   </si>
   <si>
-    <t>expected initial value expression</t>
-  </si>
-  <si>
-    <t>Extra comments (expected value in !Comments)</t>
-  </si>
-  <si>
     <t>comp</t>
   </si>
   <si>
@@ -365,9 +359,6 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>Simple volume for testing; expression for compartment evaluates to its mass</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='SpeciesType' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -452,9 +443,6 @@
     <t>molecule</t>
   </si>
   <si>
-    <t>num molecules provided in init species conc.</t>
-  </si>
-  <si>
     <t>species_2[comp]</t>
   </si>
   <si>
@@ -473,9 +461,6 @@
     <t>Species 4</t>
   </si>
   <si>
-    <t>molar conc. -&gt; molecules given by conc * vol * NA</t>
-  </si>
-  <si>
     <t>species_5[comp]</t>
   </si>
   <si>
@@ -539,9 +524,6 @@
     <t>species_4[comp] + species_5[comp]</t>
   </si>
   <si>
-    <t>Linear function of species</t>
-  </si>
-  <si>
     <t>observable_6</t>
   </si>
   <si>
@@ -554,9 +536,6 @@
     <t>observable_4 + species_5[comp]</t>
   </si>
   <si>
-    <t>Expression of other observable and species</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='Function' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -575,63 +554,39 @@
     <t>gram liter^-1</t>
   </si>
   <si>
-    <t>Uses a Parameter</t>
-  </si>
-  <si>
     <t>function_4</t>
   </si>
   <si>
     <t>species_1[comp] + species_2[comp]</t>
   </si>
   <si>
-    <t>Uses a Species</t>
-  </si>
-  <si>
     <t>function_5</t>
   </si>
   <si>
-    <t>Uses an Observable</t>
-  </si>
-  <si>
     <t>function_6</t>
   </si>
   <si>
     <t>function_1 + function_2</t>
   </si>
   <si>
-    <t>Uses another Function</t>
-  </si>
-  <si>
     <t>function_7</t>
   </si>
   <si>
-    <t>Uses a 'Compartment', i.e., its mass</t>
-  </si>
-  <si>
     <t>function_9</t>
   </si>
   <si>
-    <t>Uses another function, a Species, &amp; an Observable</t>
-  </si>
-  <si>
     <t>volume_comp</t>
   </si>
   <si>
     <t>comp / density_comp</t>
   </si>
   <si>
-    <t>Uses the compartment mass and a Parameter</t>
-  </si>
-  <si>
     <t>function_8</t>
   </si>
   <si>
     <t>density_comp * volume_comp + comp</t>
   </si>
   <si>
-    <t>Uses a Parameter, another Function, &amp; a Compartment, and</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='Reaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -731,9 +686,6 @@
     <t>k_cat_1</t>
   </si>
   <si>
-    <t>Uses Parameter</t>
-  </si>
-  <si>
     <t>reaction_2-forward</t>
   </si>
   <si>
@@ -752,9 +704,6 @@
     <t>k_cat_3 * species_1[comp]</t>
   </si>
   <si>
-    <t>Uses Parameter &amp; Species</t>
-  </si>
-  <si>
     <t>reaction_4-forward</t>
   </si>
   <si>
@@ -764,9 +713,6 @@
     <t>k_cat_4 * observable_4</t>
   </si>
   <si>
-    <t>Uses Parameter &amp; Observable</t>
-  </si>
-  <si>
     <t>reaction_5-forward</t>
   </si>
   <si>
@@ -776,9 +722,6 @@
     <t>function_4 / k_cat_5</t>
   </si>
   <si>
-    <t>Uses Parameter &amp; Function</t>
-  </si>
-  <si>
     <t>reaction_6-forward</t>
   </si>
   <si>
@@ -788,9 +731,6 @@
     <t>k_cat_6 * comp</t>
   </si>
   <si>
-    <t>Uses Parameter &amp; Compartment</t>
-  </si>
-  <si>
     <t>reaction_7-forward</t>
   </si>
   <si>
@@ -800,9 +740,6 @@
     <t>k_cat_3 * species_1[comp] + k_cat_4 * observable_4 + function_4 / k_cat_5 + k_cat_6 * comp</t>
   </si>
   <si>
-    <t>uses Parameter, Species, Observable, Function, &amp; Compartment</t>
-  </si>
-  <si>
     <t>reaction_8-forward</t>
   </si>
   <si>
@@ -812,9 +749,6 @@
     <t>k_cat_10 * volume_comp</t>
   </si>
   <si>
-    <t>Uses Parameters and compartment volume function</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='DfbaObjective' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -878,9 +812,6 @@
     <t>Fraction of cell mass which is non water</t>
   </si>
   <si>
-    <t>[Ref-0006]</t>
-  </si>
-  <si>
     <t>k_cat</t>
   </si>
   <si>
@@ -929,12 +860,6 @@
     <t>molecule mol^-1</t>
   </si>
   <si>
-    <t>As defined at the 26th BIPM Conference, May 2019</t>
-  </si>
-  <si>
-    <t>In test DynamicExpressions model</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -974,18 +899,12 @@
     <t>0.4 &lt; function_6 &lt;= 10</t>
   </si>
   <si>
-    <t>Uses a Function</t>
-  </si>
-  <si>
     <t>stop_condition_7</t>
   </si>
   <si>
     <t>comp &lt; k_cat_9</t>
   </si>
   <si>
-    <t>Uses a 'Compartment', i.e., its mass; sum over species</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -1146,6 +1065,24 @@
   </si>
   <si>
     <t>function_5 + species_2[comp]</t>
+  </si>
+  <si>
+    <t>reaction_9</t>
+  </si>
+  <si>
+    <t>reaction name 9</t>
+  </si>
+  <si>
+    <t>[comp]: species_1 ==&gt; species_1 + species_6</t>
+  </si>
+  <si>
+    <t>reaction_9-forward</t>
+  </si>
+  <si>
+    <t>Rate law 9</t>
+  </si>
+  <si>
+    <t>No expressions depend on this reaction</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1198,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1329,20 +1266,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1350,6 +1277,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1983,17 +1913,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3:H9"/>
     </sheetView>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2006,20 +1936,17 @@
     <col min="6" max="6" width="9.6640625" style="17" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="17" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.6640625" style="17" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="17" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="17" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="17"/>
+    <col min="9" max="1024" width="8.83203125" style="17" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="17" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2027,7 +1954,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>79</v>
@@ -2047,143 +1974,85 @@
       <c r="I2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="22">
-        <v>1000000000</v>
-      </c>
-      <c r="J3" s="17">
-        <f>'!!Initial species concentration'!E3</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
+      <c r="D7" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="22">
-        <v>2000000000</v>
-      </c>
-      <c r="J4" s="17">
-        <f>'!!Initial species concentration'!E4</f>
-        <v>2000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="22">
-        <v>3000000000</v>
-      </c>
-      <c r="J5" s="17">
-        <f>'!!Initial species concentration'!E5</f>
-        <v>3000000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+      <c r="D8" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="17">
-        <v>481771260.80000001</v>
-      </c>
-      <c r="J6" s="24">
-        <f>'!!Initial species concentration'!E6*'!!Compartments'!I4*'!!Parameters'!D14</f>
-        <v>481771260.80000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+      <c r="C9" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="17">
-        <v>1083985336.8</v>
-      </c>
-      <c r="J7" s="24">
-        <f>J6 + '!!Initial species concentration'!E7*'!!Compartments'!I4*'!!Parameters'!D14</f>
-        <v>1083985336.8</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="17">
-        <v>4000000000</v>
-      </c>
-      <c r="J8" s="17">
-        <f>2 * J4</f>
-        <v>4000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="17">
-        <v>1083985336.8</v>
-      </c>
-      <c r="J9" s="24">
-        <f>J6 + '!!Initial species concentration'!E7*'!!Compartments'!I4*'!!Parameters'!D14</f>
-        <v>1083985336.8</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>156</v>
+      <c r="D9" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2194,14 +2063,14 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3:H12"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A10" sqref="A10:XFD10"/>
@@ -2209,29 +2078,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="30" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="30" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="30" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="30" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="22.1640625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="46.83203125" style="30" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="30" customWidth="1"/>
-    <col min="13" max="1026" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="30" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="13.83203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="26" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="26" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="26" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="26" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="26" customWidth="1"/>
+    <col min="11" max="1024" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2239,7 +2106,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>79</v>
@@ -2259,219 +2126,120 @@
       <c r="I2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="26">
-        <f>0.1</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="26">
-        <f>0.5 / EXP(0)</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="30" t="s">
+      <c r="D9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="H5" s="30">
-        <v>1100</v>
-      </c>
-      <c r="J5" s="26">
-        <f>'!!Parameters'!D15</f>
-        <v>1100</v>
-      </c>
-      <c r="K5" s="30" t="s">
+      <c r="C10" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="C11" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="D11" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="30">
-        <v>3000000000</v>
-      </c>
-      <c r="J6" s="26">
-        <f>'!!Initial species concentration'!E3 + '!!Initial species concentration'!E4</f>
-        <v>3000000000</v>
-      </c>
-      <c r="K6" s="30" t="s">
+      <c r="C12" s="26" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="30">
-        <v>3000000000</v>
-      </c>
-      <c r="J7" s="26">
-        <f>'!!Observables'!J5</f>
-        <v>3000000000</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" s="30">
-        <v>0.6</v>
-      </c>
-      <c r="J8" s="26">
-        <f>J3+J4</f>
-        <v>0.6</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J9" s="27">
-        <f>'!!Compartments'!V4</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H10" s="30">
-        <v>2000000000</v>
-      </c>
-      <c r="J10" s="26">
-        <f>'!!Observables'!J5 - J7 + '!!Initial species concentration'!E4</f>
-        <v>2000000000</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="30">
-        <v>2E-3</v>
-      </c>
-      <c r="J11" s="27">
-        <f>'!!Compartments'!V4 / '!!Parameters'!D15</f>
-        <v>2E-3</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="30">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J12" s="27">
-        <f>'!!Parameters'!D15 * J11+ '!!Compartments'!V4</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>181</v>
+      <c r="D12" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2482,14 +2250,14 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
       <selection activeCell="D9" sqref="D9"/>
@@ -2497,16 +2265,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="30" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="42" style="30" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="30" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="12" style="26" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="42" style="26" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="26" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="26" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="14" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="30" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="26" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="26" customWidth="1"/>
     <col min="11" max="12" width="8.83203125" style="14" customWidth="1"/>
     <col min="13" max="13" width="37.33203125" style="14" customWidth="1"/>
     <col min="14" max="1027" width="8.83203125" style="14" customWidth="1"/>
@@ -2516,21 +2284,21 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
+      <c r="G2" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2545,22 +2313,22 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>79</v>
@@ -2582,176 +2350,199 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="A4" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="30">
+      <c r="D4" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="26">
         <v>0</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>193</v>
+      <c r="F4" s="26" t="s">
+        <v>178</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="E5" s="30">
+      <c r="D5" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="E5" s="26">
         <v>0</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="F5" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="14"/>
       <c r="J5" s="23"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>349</v>
+      <c r="D6" s="26" t="s">
+        <v>322</v>
       </c>
       <c r="E6" s="14">
         <v>0</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>193</v>
+      <c r="F6" s="26" t="s">
+        <v>178</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="30">
+        <v>177</v>
+      </c>
+      <c r="E7" s="26">
         <v>0</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>193</v>
+      <c r="F7" s="26" t="s">
+        <v>178</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="30" t="s">
+      <c r="A8" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>352</v>
-      </c>
-      <c r="E8" s="30">
+        <v>325</v>
+      </c>
+      <c r="E8" s="26">
         <v>0</v>
       </c>
-      <c r="F8" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>351</v>
+      <c r="F8" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" s="30" t="s">
+      <c r="A9" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>350</v>
-      </c>
-      <c r="E9" s="30">
+      <c r="D9" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="E9" s="26">
         <v>0</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>193</v>
+      <c r="F9" s="26" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="30" t="s">
+      <c r="A10" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="26">
+        <v>0</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="E10" s="30">
+      <c r="C11" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="26">
         <v>0</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="F11" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="C12" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="30">
+      <c r="D12" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="E12" s="28">
         <v>0</v>
       </c>
-      <c r="F11" s="30" t="s">
-        <v>193</v>
+      <c r="F12" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2766,43 +2557,41 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3:K11"/>
     </sheetView>
-    <sheetView topLeftCell="B2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" style="30" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="30" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.83203125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="30" customWidth="1"/>
-    <col min="8" max="10" width="9.1640625" style="30" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="28" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="28" customWidth="1"/>
-    <col min="14" max="14" width="52.1640625" style="30" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1026" max="1028" width="9" style="30" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="19" style="26" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="26" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="26" customWidth="1"/>
+    <col min="8" max="10" width="9.1640625" style="26" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="13" max="1023" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1024" max="1026" width="9" style="26" customWidth="1"/>
+    <col min="1027" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2810,16 +2599,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>79</v>
@@ -2839,252 +2628,191 @@
       <c r="L2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="G7" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B8" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="C8" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="G3" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K3" s="28">
-        <v>1</v>
-      </c>
-      <c r="M3" s="28">
-        <f>'!!Parameters'!J4</f>
-        <v>1</v>
-      </c>
-      <c r="N3" s="30" t="s">
+      <c r="G8" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="B9" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="C9" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F4" s="30" t="s">
+      <c r="G9" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K4" s="28">
-        <v>0.2</v>
-      </c>
-      <c r="M4" s="28">
-        <f>'!!Parameters'!J5/10</f>
-        <v>0.2</v>
-      </c>
-      <c r="N4" s="30" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C10" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K5" s="28">
-        <v>3000000000</v>
-      </c>
-      <c r="M5" s="28">
-        <f>'!!Parameters'!J6 * '!!Initial species concentration'!E3</f>
-        <v>3000000000</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>223</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="G10" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K6" s="28">
-        <v>1927085043.2</v>
-      </c>
-      <c r="M6" s="29">
-        <f>'!!Parameters'!J7 * '!!Observables'!J6</f>
-        <v>1927085043.2</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K7" s="28">
-        <v>600000000</v>
-      </c>
-      <c r="M7" s="29">
-        <f>'!!Functions'!J6 / '!!Parameters'!J8</f>
-        <v>600000000</v>
-      </c>
-      <c r="N7" s="30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>231</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K8" s="28">
-        <v>13.2</v>
-      </c>
-      <c r="M8" s="29">
-        <f>'!!Parameters'!J9 * '!!Compartments'!V4</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="N8" s="30" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K9" s="28">
-        <v>5527085056.3999996</v>
-      </c>
-      <c r="M9" s="29">
-        <f>M5 + M6 + M7 + M8</f>
-        <v>5527085056.3999996</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="K10" s="28">
-        <v>0.02</v>
-      </c>
-      <c r="M10" s="29">
-        <f>'!!Parameters'!D13 * '!!Functions'!J11</f>
-        <v>0.02</v>
-      </c>
-      <c r="N10" s="30" t="s">
-        <v>242</v>
-      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="L11" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3109,23 +2837,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="11" style="30" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" style="30" customWidth="1"/>
-    <col min="8" max="9" width="9" style="30" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="30" hidden="1"/>
-    <col min="11" max="11" width="15" style="30" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="9" style="30" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="27.33203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="11" style="26" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.1640625" style="26" customWidth="1"/>
+    <col min="8" max="9" width="9" style="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" style="26" hidden="1"/>
+    <col min="11" max="11" width="15" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="26" customWidth="1"/>
+    <col min="13" max="13" width="9" style="26" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3136,19 +2864,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>79</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -3168,21 +2896,21 @@
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="G3" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3220,7 +2948,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3231,13 +2959,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>44</v>
@@ -3257,22 +2985,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3305,17 +3033,17 @@
     <col min="5" max="5" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="8" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="30" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="30"/>
+    <col min="8" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="12" max="1026" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1027" max="1029" width="9" style="26" customWidth="1"/>
+    <col min="1030" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3326,13 +3054,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>79</v>
@@ -3355,45 +3083,45 @@
     </row>
     <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>127</v>
+        <v>225</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="E3" s="10">
         <v>-3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>130</v>
+        <v>225</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>125</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3404,14 +3132,14 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3:J15"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="F18" sqref="F18"/>
@@ -3419,27 +3147,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="30" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="30" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="30" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="30" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="26" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="26" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="46.5" style="6" customWidth="1"/>
-    <col min="14" max="1026" width="8.83203125" style="6" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="6" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="6"/>
+    <col min="12" max="1024" width="8.83203125" style="6" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="6" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3447,13 +3173,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>79</v>
@@ -3473,275 +3199,233 @@
       <c r="K2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="30" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="30">
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="26">
         <v>0.3</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="M3" s="30" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D4" s="30">
+      <c r="F3" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="26">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="26">
         <v>0</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="J4" s="30">
-        <v>1</v>
-      </c>
-      <c r="M4" s="30"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D5" s="30">
+      <c r="F4" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="26">
         <v>2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="26">
         <v>0</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="J5" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D6" s="30">
+      <c r="F5" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="26">
         <v>3</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="26">
         <v>0</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="J6" s="30">
+      <c r="F6" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="26">
+        <v>4</v>
+      </c>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="26">
+        <v>5</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" s="26">
+        <v>6</v>
+      </c>
+      <c r="E9" s="26">
+        <v>0</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="26">
+        <v>7</v>
+      </c>
+      <c r="E10" s="26">
+        <v>0</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="26">
+        <v>1000000000</v>
+      </c>
+      <c r="E11" s="26">
+        <v>0</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" s="26">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="30">
-        <v>4</v>
-      </c>
-      <c r="E7" s="30">
+      <c r="E12" s="26">
         <v>0</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="J7" s="30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" s="30">
-        <v>5</v>
-      </c>
-      <c r="E8" s="30">
+      <c r="F12" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" s="26">
+        <v>10</v>
+      </c>
+      <c r="E13" s="26">
         <v>0</v>
       </c>
-      <c r="F8" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="J8" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" s="30">
-        <v>6</v>
-      </c>
-      <c r="E9" s="30">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="J9" s="30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D10" s="30">
-        <v>7</v>
-      </c>
-      <c r="E10" s="30">
-        <v>0</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="30">
-        <v>1000000000</v>
-      </c>
-      <c r="E11" s="30">
-        <v>0</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="J11" s="30">
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D12" s="30">
-        <v>3</v>
-      </c>
-      <c r="E12" s="30">
-        <v>0</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="D13" s="30">
-        <v>10</v>
-      </c>
-      <c r="E13" s="30">
-        <v>0</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="J13" s="30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="30" t="s">
-        <v>279</v>
+      <c r="F13" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="26" t="s">
+        <v>256</v>
       </c>
       <c r="D14" s="7">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="26">
         <v>0</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="J14" s="7">
-        <v>6.0221407599999999E+23</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="30">
+      <c r="F14" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="26">
         <v>1100</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="26">
         <v>0</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="J15" s="30">
-        <v>1100</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F15" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -3819,42 +3503,40 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M16" sqref="M16"/>
       <selection pane="topRight" activeCell="M16" sqref="M16"/>
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="30" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="30" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="30" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="30" customWidth="1"/>
-    <col min="11" max="11" width="33" style="30" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="30" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="20" style="26" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="26" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="26" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="26" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="26" customWidth="1"/>
+    <col min="10" max="1024" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3862,7 +3544,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>79</v>
@@ -3882,153 +3564,84 @@
       <c r="I2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>284</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>285</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="30" t="b">
-        <f>IF(0 &lt; 1, TRUE())</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>287</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="30" t="b">
-        <f>IF(2 &lt;  1, TRUE())</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="30" t="b">
-        <f>IF('!!Parameters'!D10=3, TRUE())</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>290</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="30" t="b">
-        <f>IF( '!!Parameters'!D11 &lt;= '!!Initial species concentration'!E3, TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="s">
-        <v>292</v>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="26" t="s">
+        <v>267</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="30" t="b">
-        <f>IF( '!!Observables'!H5 &lt;= '!!Initial species concentration'!E3, TRUE())</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>295</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="30" t="b">
-        <f>IF( AND(0.4 &lt; '!!Functions'!J8,  '!!Functions'!J8 &lt;= 10), TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>297</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="30" t="b">
-        <f>IF( '!!Compartments'!V4 &lt; '!!Parameters'!D12, TRUE())</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>299</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4051,36 +3664,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="30"/>
+    <col min="1" max="3" width="9" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="Q2" s="37" t="s">
-        <v>303</v>
-      </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="37" t="s">
-        <v>304</v>
-      </c>
-      <c r="T2" s="33"/>
+      <c r="G2" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="H2" s="30"/>
+      <c r="I2" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="Q2" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="R2" s="30"/>
+      <c r="S2" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="T2" s="30"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4090,22 +3703,22 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>57</v>
@@ -4117,19 +3730,19 @@
         <v>70</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>31</v>
@@ -4177,11 +3790,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1026" max="1028" width="9" style="30" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="8.83203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="75.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1026" max="1028" width="9" style="26" customWidth="1"/>
+    <col min="1029" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -4193,7 +3806,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4201,7 +3814,7 @@
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4209,7 +3822,7 @@
       <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="26" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4217,7 +3830,7 @@
       <c r="A5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4225,7 +3838,7 @@
       <c r="A6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4233,7 +3846,7 @@
       <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4241,7 +3854,7 @@
       <c r="A8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="26" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4249,7 +3862,7 @@
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4297,15 +3910,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="30" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" style="30" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="14" style="26" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" style="26" customWidth="1"/>
+    <col min="4" max="6" width="9.1640625" style="26" customWidth="1"/>
     <col min="7" max="1017" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4316,7 +3929,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -4360,22 +3973,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="30" customWidth="1"/>
-    <col min="3" max="14" width="9.1640625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="26" customWidth="1"/>
+    <col min="3" max="14" width="9.1640625" style="26" customWidth="1"/>
     <col min="15" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="37" t="s">
-        <v>315</v>
-      </c>
-      <c r="H2" s="33"/>
+      <c r="G2" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4385,16 +3998,16 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>31</v>
@@ -4415,10 +4028,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4489,7 +4102,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4500,46 +4113,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>320</v>
+        <v>293</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>44</v>
@@ -4570,13 +4183,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="30"/>
+    <col min="1" max="3" width="9" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4587,28 +4200,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4636,13 +4249,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="30"/>
+    <col min="1" max="3" width="9" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -4653,28 +4266,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4692,10 +4305,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4716,11 +4329,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="34" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1026" max="1028" width="9" style="30" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="8.83203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="34" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1026" max="1028" width="9" style="26" customWidth="1"/>
+    <col min="1029" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -4732,7 +4345,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4740,7 +4353,7 @@
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4748,7 +4361,7 @@
       <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="26" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4761,7 +4374,7 @@
       <c r="A6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4789,8 +4402,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="30" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="26" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="26" customWidth="1"/>
     <col min="3" max="1015" width="8.83203125" style="12" customWidth="1"/>
     <col min="1016" max="1018" width="9" style="12" customWidth="1"/>
     <col min="1019" max="16384" width="9" style="12"/>
@@ -4805,7 +4418,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4818,7 +4431,7 @@
       <c r="A4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="26">
         <v>37</v>
       </c>
     </row>
@@ -4826,7 +4439,7 @@
       <c r="A5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4913,7 +4526,7 @@
       <c r="B3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="26" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="11"/>
@@ -4922,7 +4535,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="30"/>
+      <c r="C4" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4932,14 +4545,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMR4"/>
+  <dimension ref="A1:AMP4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
     <sheetView topLeftCell="F1" workbookViewId="1">
       <selection activeCell="W5" sqref="W5"/>
@@ -4947,30 +4560,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="30" customWidth="1"/>
-    <col min="2" max="3" width="16.1640625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="16" style="30" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="8" style="30" customWidth="1"/>
-    <col min="8" max="16" width="8.83203125" style="30" customWidth="1"/>
-    <col min="17" max="18" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="30" customWidth="1"/>
-    <col min="20" max="20" width="12.5" style="30" customWidth="1"/>
-    <col min="21" max="21" width="8.83203125" style="30" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="8.83203125" style="30" customWidth="1"/>
-    <col min="23" max="23" width="33.1640625" style="30" customWidth="1"/>
-    <col min="24" max="1035" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1036" max="1038" width="9" style="30" customWidth="1"/>
-    <col min="1039" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="7.33203125" style="26" customWidth="1"/>
+    <col min="2" max="3" width="16.1640625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="16" style="26" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="8" style="26" customWidth="1"/>
+    <col min="8" max="16" width="8.83203125" style="26" customWidth="1"/>
+    <col min="17" max="18" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="26" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="1033" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1034" max="1036" width="9" style="26" customWidth="1"/>
+    <col min="1037" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1032" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1030" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:1032" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -4978,19 +4588,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -6005,10 +5615,8 @@
       <c r="AMN2" s="15"/>
       <c r="AMO2" s="15"/>
       <c r="AMP2" s="15"/>
-      <c r="AMQ2" s="15"/>
-      <c r="AMR2" s="15"/>
-    </row>
-    <row r="3" spans="1:1032" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:1030" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -6072,12 +5680,8 @@
       <c r="U3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>82</v>
-      </c>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
@@ -7085,64 +6689,52 @@
       <c r="AMN3" s="15"/>
       <c r="AMO3" s="15"/>
       <c r="AMP3" s="15"/>
-      <c r="AMQ3" s="15"/>
-      <c r="AMR3" s="15"/>
-    </row>
-    <row r="4" spans="1:1032" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    </row>
+    <row r="4" spans="1:1030" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="D4" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="H4" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="I4" s="7">
         <v>2E-3</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="26">
         <v>0</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="N4" s="26">
+        <v>7.75</v>
+      </c>
+      <c r="O4" s="26">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="P4" s="26" t="s">
         <v>90</v>
-      </c>
-      <c r="L4" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M4" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="N4" s="30">
-        <v>7.75</v>
-      </c>
-      <c r="O4" s="30">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="P4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="T4" s="30">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="V4" s="7">
-        <f>I4 * '!!Parameters'!D15</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="W4" s="30" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -7165,42 +6757,42 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="30" customWidth="1"/>
-    <col min="2" max="2" width="15" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="30" customWidth="1"/>
-    <col min="8" max="8" width="7" style="30" customWidth="1"/>
-    <col min="9" max="9" width="14" style="30" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="30" customWidth="1"/>
-    <col min="11" max="12" width="8.6640625" style="30" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="30" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="30" customWidth="1"/>
-    <col min="15" max="1028" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1029" max="1031" width="9" style="30" customWidth="1"/>
-    <col min="1032" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="9" style="26" customWidth="1"/>
+    <col min="2" max="2" width="15" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="26" customWidth="1"/>
+    <col min="8" max="8" width="7" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14" style="26" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="26" customWidth="1"/>
+    <col min="11" max="12" width="8.6640625" style="26" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="26" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="26" customWidth="1"/>
+    <col min="15" max="1028" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1029" max="1031" width="9" style="26" customWidth="1"/>
+    <col min="1032" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -7210,25 +6802,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>102</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>44</v>
@@ -7247,110 +6839,110 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="26">
+        <v>0</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="30">
-        <v>1</v>
-      </c>
-      <c r="H4" s="30">
+      <c r="G5" s="26">
+        <v>2</v>
+      </c>
+      <c r="H5" s="26">
         <v>0</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="G6" s="26">
+        <v>3</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="30">
-        <v>2</v>
-      </c>
-      <c r="H5" s="30">
+      <c r="B7" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="26">
+        <v>4</v>
+      </c>
+      <c r="H7" s="26">
         <v>0</v>
       </c>
-      <c r="I5" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="30" t="s">
+      <c r="I7" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="G6" s="30">
-        <v>3</v>
-      </c>
-      <c r="H6" s="30">
+      <c r="B8" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="26">
+        <v>5</v>
+      </c>
+      <c r="H8" s="26">
         <v>0</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="I8" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="30">
-        <v>4</v>
-      </c>
-      <c r="H7" s="30">
+      <c r="B9" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="26">
+        <v>6</v>
+      </c>
+      <c r="H9" s="26">
         <v>0</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" s="30">
-        <v>5</v>
-      </c>
-      <c r="H8" s="30">
-        <v>0</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="G9" s="30">
-        <v>6</v>
-      </c>
-      <c r="H9" s="30">
-        <v>0</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>105</v>
+      <c r="I9" s="26" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -7365,14 +6957,14 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3:K8"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3:I8"/>
     </sheetView>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
       <selection activeCell="K7" sqref="K7"/>
@@ -7380,29 +6972,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" style="30" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="30" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="30" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="30" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="30" customWidth="1"/>
-    <col min="12" max="12" width="50.33203125" style="30" customWidth="1"/>
-    <col min="13" max="1026" width="9.1640625" style="30" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="30" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="18" style="26" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="26" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="26" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="26" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="26" hidden="1" customWidth="1"/>
+    <col min="11" max="1024" width="9.1640625" style="26" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -7410,10 +7000,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>79</v>
@@ -7433,168 +7023,120 @@
       <c r="J2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="18" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="E3" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C4" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="30" t="s">
+      <c r="D4" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="28">
-        <v>1000000000</v>
-      </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28">
-        <f>'!!Initial species concentration'!E3</f>
-        <v>1000000000</v>
-      </c>
-      <c r="L3" s="30" t="s">
+      <c r="B5" s="26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="C5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I4" s="28">
-        <v>2000000000</v>
-      </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28">
-        <f>'!!Initial species concentration'!E4</f>
-        <v>2000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+      <c r="C6" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="28">
-        <v>3000000000</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28">
-        <f>'!!Initial species concentration'!E5</f>
-        <v>3000000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="C7" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B8" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I6" s="28">
-        <v>481771260.80000001</v>
-      </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28">
-        <f>'!!Initial species concentration'!E6 * vol_comp * NA</f>
-        <v>481771260.80000001</v>
-      </c>
-      <c r="L6" s="30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="28">
-        <v>602214076</v>
-      </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28">
-        <f>'!!Initial species concentration'!E7 * vol_comp * NA</f>
-        <v>602214076</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="28">
-        <v>722656891.19999993</v>
-      </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28">
-        <f>'!!Initial species concentration'!E8 * vol_comp * NA</f>
-        <v>722656891.19999993</v>
-      </c>
+      <c r="C8" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -7615,7 +7157,7 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
       <selection activeCell="H1" sqref="H1:H1048576"/>
@@ -7623,25 +7165,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" style="30" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="30" customWidth="1"/>
-    <col min="3" max="3" width="19" style="30" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="30" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="30" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="8.6640625" style="30" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="30" customWidth="1"/>
-    <col min="13" max="1026" width="8.83203125" style="30" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="30" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="30"/>
+    <col min="1" max="1" width="27" style="26" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="19" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="26" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="26" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="26" customWidth="1"/>
+    <col min="13" max="1026" width="8.83203125" style="26" customWidth="1"/>
+    <col min="1027" max="1029" width="9" style="26" customWidth="1"/>
+    <col min="1030" max="16384" width="9" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -7652,7 +7194,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>76</v>
@@ -7683,123 +7225,123 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>89</v>
+      <c r="A3" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E3" s="22">
         <v>1000000000</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="26">
         <v>0</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>89</v>
+      <c r="A4" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E4" s="22">
         <v>2000000000</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="26">
         <v>0</v>
       </c>
       <c r="G4" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>89</v>
+      <c r="D5" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E5" s="22">
         <v>3000000000</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="26">
         <v>0</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>89</v>
+      <c r="A6" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E6" s="22">
         <v>4.0000000000000001E-13</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="26">
         <v>0</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>89</v>
+      <c r="A7" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E7" s="22">
         <v>4.9999999999999999E-13</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="26">
         <v>0</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>89</v>
+      <c r="A8" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>87</v>
       </c>
       <c r="E8" s="22">
         <v>5.9999999999999997E-13</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="26">
         <v>0</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify for test simulation: make stop conditions fail at time 0; slow down rates of overly fast reactions
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30900" yWindow="2100" windowWidth="29020" windowHeight="17400" tabRatio="993" firstSheet="2" activeTab="11"/>
-    <workbookView xWindow="820" yWindow="4560" windowWidth="31800" windowHeight="14380" tabRatio="500" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="-31620" yWindow="1340" windowWidth="29020" windowHeight="17400" tabRatio="993" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="780" yWindow="3000" windowWidth="29180" windowHeight="14080" tabRatio="500" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="335">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -701,27 +701,18 @@
     <t>Rate law 3</t>
   </si>
   <si>
-    <t>k_cat_3 * species_1[comp]</t>
-  </si>
-  <si>
     <t>reaction_4-forward</t>
   </si>
   <si>
     <t>Rate law 4</t>
   </si>
   <si>
-    <t>k_cat_4 * observable_4</t>
-  </si>
-  <si>
     <t>reaction_5-forward</t>
   </si>
   <si>
     <t>Rate law 5</t>
   </si>
   <si>
-    <t>function_4 / k_cat_5</t>
-  </si>
-  <si>
     <t>reaction_6-forward</t>
   </si>
   <si>
@@ -737,9 +728,6 @@
     <t>Rate law 7</t>
   </si>
   <si>
-    <t>k_cat_3 * species_1[comp] + k_cat_4 * observable_4 + function_4 / k_cat_5 + k_cat_6 * comp</t>
-  </si>
-  <si>
     <t>reaction_8-forward</t>
   </si>
   <si>
@@ -866,9 +854,6 @@
     <t>stop_condition_1</t>
   </si>
   <si>
-    <t>0 &lt; 1</t>
-  </si>
-  <si>
     <t>stop_condition_2</t>
   </si>
   <si>
@@ -890,21 +875,12 @@
     <t>stop_condition_5</t>
   </si>
   <si>
-    <t>observable_3 &lt; species_1[comp]</t>
-  </si>
-  <si>
     <t>stop_condition_6</t>
   </si>
   <si>
-    <t>0.4 &lt; function_6 &lt;= 10</t>
-  </si>
-  <si>
     <t>stop_condition_7</t>
   </si>
   <si>
-    <t>comp &lt; k_cat_9</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -1083,6 +1059,36 @@
   </si>
   <si>
     <t>No expressions depend on this reaction</t>
+  </si>
+  <si>
+    <t>2 * observable_3 &lt; species_1[comp]</t>
+  </si>
+  <si>
+    <t>1.0 &lt; function_6 &lt;= 10</t>
+  </si>
+  <si>
+    <t>0 == 1</t>
+  </si>
+  <si>
+    <t>k_cat_9 &lt; comp</t>
+  </si>
+  <si>
+    <t>scaling_factor</t>
+  </si>
+  <si>
+    <t>factor to slow down overly fast reactions</t>
+  </si>
+  <si>
+    <t>scaling_factor * k_cat_3 * species_1[comp]</t>
+  </si>
+  <si>
+    <t>scaling_factor * k_cat_4 * observable_4</t>
+  </si>
+  <si>
+    <t>scaling_factor * (k_cat_3 * species_1[comp] + k_cat_4 * observable_4 + function_4 / k_cat_5 + k_cat_6 * comp)</t>
+  </si>
+  <si>
+    <t>scaling_factor * function_4 / k_cat_5</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1204,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1281,6 +1287,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1298,6 +1307,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1920,7 +1932,7 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3:H9"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="C14" sqref="C14"/>
@@ -2070,7 +2082,7 @@
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3:H12"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
       <selection activeCell="A10" sqref="A10:XFD10"/>
@@ -2214,7 +2226,7 @@
         <v>162</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>118</v>
@@ -2252,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
@@ -2294,11 +2306,11 @@
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2382,7 +2394,7 @@
         <v>64</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E5" s="26">
         <v>0</v>
@@ -2406,7 +2418,7 @@
         <v>64</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E6" s="14">
         <v>0</v>
@@ -2450,7 +2462,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E8" s="26">
         <v>0</v>
@@ -2459,7 +2471,7 @@
         <v>178</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2473,7 +2485,7 @@
         <v>64</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="E9" s="26">
         <v>0</v>
@@ -2524,16 +2536,16 @@
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="E12" s="28">
         <v>0</v>
@@ -2542,7 +2554,7 @@
         <v>178</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2559,14 +2571,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3:K11"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2683,7 +2695,7 @@
         <v>198</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>205</v>
+        <v>331</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>178</v>
@@ -2691,10 +2703,10 @@
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="26" t="s">
         <v>206</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>207</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>183</v>
@@ -2703,7 +2715,7 @@
         <v>198</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>208</v>
+        <v>332</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>178</v>
@@ -2711,10 +2723,10 @@
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>185</v>
@@ -2723,7 +2735,7 @@
         <v>198</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>211</v>
+        <v>334</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>178</v>
@@ -2731,10 +2743,10 @@
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>187</v>
@@ -2743,7 +2755,7 @@
         <v>198</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G8" s="26" t="s">
         <v>178</v>
@@ -2751,10 +2763,10 @@
     </row>
     <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>189</v>
@@ -2763,7 +2775,7 @@
         <v>198</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>217</v>
+        <v>333</v>
       </c>
       <c r="G9" s="26" t="s">
         <v>178</v>
@@ -2771,10 +2783,10 @@
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>191</v>
@@ -2783,7 +2795,7 @@
         <v>198</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>178</v>
@@ -2791,20 +2803,20 @@
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>198</v>
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G11" s="28" t="s">
         <v>178</v>
@@ -2853,7 +2865,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -2873,10 +2885,10 @@
         <v>79</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -2896,13 +2908,13 @@
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>90</v>
@@ -2948,7 +2960,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2965,7 +2977,7 @@
         <v>79</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>44</v>
@@ -2985,10 +2997,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>64</v>
@@ -3000,7 +3012,7 @@
         <v>88</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3043,7 +3055,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3054,7 +3066,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>130</v>
@@ -3083,13 +3095,13 @@
     </row>
     <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>123</v>
@@ -3098,21 +3110,21 @@
         <v>-3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>125</v>
@@ -3121,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3135,14 +3147,14 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="J3" sqref="J3:J15"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12:F12"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3162,7 +3174,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.15">
@@ -3179,7 +3191,7 @@
         <v>93</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>79</v>
@@ -3202,10 +3214,10 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D3" s="26">
         <v>0.3</v>
@@ -3220,7 +3232,7 @@
         <v>199</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D4" s="26">
         <v>1</v>
@@ -3235,10 +3247,10 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D5" s="26">
         <v>2</v>
@@ -3253,10 +3265,10 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D6" s="26">
         <v>3</v>
@@ -3265,16 +3277,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D7" s="26">
         <v>4</v>
@@ -3283,34 +3295,34 @@
         <v>0</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D8" s="26">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="26">
         <v>0</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D9" s="26">
         <v>6</v>
@@ -3319,16 +3331,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="26" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D10" s="26">
         <v>7</v>
@@ -3343,13 +3355,13 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="D11" s="26">
-        <v>1000000000</v>
+        <v>238</v>
+      </c>
+      <c r="D11" s="7">
+        <v>10000000000</v>
       </c>
       <c r="E11" s="26">
         <v>0</v>
@@ -3361,10 +3373,10 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D12" s="26">
         <v>3</v>
@@ -3379,10 +3391,10 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="26" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D13" s="26">
         <v>10</v>
@@ -3391,13 +3403,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="26" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D14" s="7">
         <v>6.0221407599999999E+23</v>
@@ -3406,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J14" s="7"/>
     </row>
@@ -3426,11 +3438,21 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
+      <c r="A16" s="6" t="s">
+        <v>329</v>
+      </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="36">
+        <v>9.9999999999999995E-8</v>
+      </c>
       <c r="E16" s="6"/>
+      <c r="F16" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6"/>
@@ -3513,7 +3535,7 @@
       <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3533,7 +3555,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3567,10 +3589,10 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>260</v>
+        <v>327</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>90</v>
@@ -3578,10 +3600,10 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>90</v>
@@ -3589,10 +3611,10 @@
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>90</v>
@@ -3600,10 +3622,10 @@
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>90</v>
@@ -3611,10 +3633,10 @@
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>268</v>
+        <v>325</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>90</v>
@@ -3622,10 +3644,10 @@
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>90</v>
@@ -3633,10 +3655,10 @@
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>272</v>
+        <v>328</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>90</v>
@@ -3670,30 +3692,30 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="Q2" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="T2" s="30"/>
+      <c r="G2" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="Q2" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="R2" s="31"/>
+      <c r="S2" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -3706,7 +3728,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>79</v>
@@ -3715,10 +3737,10 @@
         <v>99</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>57</v>
@@ -3730,19 +3752,19 @@
         <v>70</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>31</v>
@@ -3918,7 +3940,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3929,7 +3951,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -3981,14 +4003,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="H2" s="30"/>
+      <c r="G2" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4001,7 +4023,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>79</v>
@@ -4028,10 +4050,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4102,7 +4124,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4113,46 +4135,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>99</v>
       </c>
       <c r="H2" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>296</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>304</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>44</v>
@@ -4189,7 +4211,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4200,28 +4222,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4255,7 +4277,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -4269,25 +4291,25 @@
         <v>99</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4305,10 +4327,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -4588,19 +4610,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -6785,14 +6807,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -7157,7 +7179,7 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
       <selection activeCell="H1" sqref="H1:H1048576"/>

</xml_diff>

<commit_message>
finish expression caching; properly invalidate cached expression values that depend on a continuous (ODE) submodel; incorporate dependencies on a Compartment expression, i.e., its mass; add flush (invalidation) operations to DynamicModel; measure cache and flush hits and hit ratios
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31620" yWindow="1340" windowWidth="29020" windowHeight="17400" tabRatio="993" firstSheet="6" activeTab="12"/>
-    <workbookView xWindow="780" yWindow="3000" windowWidth="29180" windowHeight="14080" tabRatio="500" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="29800" windowHeight="15300" tabRatio="993" firstSheet="6" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="352">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -278,18 +277,9 @@
     <t>!Conclusions</t>
   </si>
   <si>
-    <t>test_submodel</t>
-  </si>
-  <si>
-    <t>Submodel with all DynamicExpressions</t>
-  </si>
-  <si>
     <t>deterministic_simulation_algorithm</t>
   </si>
   <si>
-    <t>Do not plan to simulate, but deterministic_simulation_algorithm would make simulation deterministic</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='Compartment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
   </si>
   <si>
@@ -746,9 +736,6 @@
     <t>!Coefficient units</t>
   </si>
   <si>
-    <t>dfba-obj-test_submodel</t>
-  </si>
-  <si>
     <t>Metabolism_biomass</t>
   </si>
   <si>
@@ -1089,6 +1076,69 @@
   </si>
   <si>
     <t>scaling_factor * function_4 / k_cat_5</t>
+  </si>
+  <si>
+    <t>deterministic_simulation_algorithm makes a simulation deterministic</t>
+  </si>
+  <si>
+    <t>ode_submodel</t>
+  </si>
+  <si>
+    <t>ordinary_differential_equations</t>
+  </si>
+  <si>
+    <t>also deterministic, but cache invalidation handled differently</t>
+  </si>
+  <si>
+    <t>dsa_submodel</t>
+  </si>
+  <si>
+    <t>dfba-obj-dsa_submodel</t>
+  </si>
+  <si>
+    <t>comp_2</t>
+  </si>
+  <si>
+    <t>Compartment with rxn that has no dependencies</t>
+  </si>
+  <si>
+    <t>species_5[comp_2]</t>
+  </si>
+  <si>
+    <t>species_6[comp_2]</t>
+  </si>
+  <si>
+    <t>Species 5 in comp 2</t>
+  </si>
+  <si>
+    <t>Species 6 in comp 2</t>
+  </si>
+  <si>
+    <t>dist-init-conc-species_5[comp_2]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-species_6[comp_2]</t>
+  </si>
+  <si>
+    <t>reaction_10</t>
+  </si>
+  <si>
+    <t>reaction name 10</t>
+  </si>
+  <si>
+    <t>[comp_2]: species_5 ==&gt; species_5 + species_6</t>
+  </si>
+  <si>
+    <t>reaction_10-forward</t>
+  </si>
+  <si>
+    <t>Rate law 10</t>
+  </si>
+  <si>
+    <t>k_cat_11</t>
+  </si>
+  <si>
+    <t>density_comp_2</t>
   </si>
 </sst>
 </file>
@@ -1199,12 +1249,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1269,9 +1320,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1289,6 +1337,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1308,13 +1371,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1656,7 +1717,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1934,9 +1994,6 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1955,7 +2012,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1966,10 +2023,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>44</v>
@@ -1989,82 +2046,82 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="26" t="s">
         <v>118</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>118</v>
+        <v>120</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>118</v>
+        <v>142</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>118</v>
+        <v>144</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>118</v>
+        <v>146</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2084,30 +2141,27 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
     </sheetView>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="26" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="26" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="26" customWidth="1"/>
-    <col min="11" max="1024" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="13.83203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="25" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -2118,10 +2172,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>44</v>
@@ -2138,120 +2192,120 @@
       <c r="I2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="26">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="C5" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="26" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="26" t="s">
+      <c r="D6" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="25" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="C7" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26" t="s">
+      <c r="D8" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>86</v>
+      <c r="C9" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>83</v>
       </c>
       <c r="H9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>86</v>
+      <c r="D12" s="25" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2262,32 +2316,30 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="26" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="42" style="26" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="26" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="12" style="25" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="14" style="25" customWidth="1"/>
+    <col min="4" max="4" width="71.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="25" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="25" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="14" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="26" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="26" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="6.5" style="25" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="5" style="14" customWidth="1"/>
     <col min="13" max="13" width="37.33203125" style="14" customWidth="1"/>
     <col min="14" max="1027" width="8.83203125" style="14" customWidth="1"/>
     <col min="1028" max="1030" width="9" style="14" customWidth="1"/>
@@ -2296,21 +2348,21 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="G2" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2325,25 +2377,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>174</v>
-      </c>
       <c r="I3" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>44</v>
@@ -2361,200 +2413,232 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:14" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="B5" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E4" s="26">
+      <c r="C5" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" s="29">
         <v>0</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F5" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="E5" s="26">
+      <c r="C6" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" s="30">
         <v>0</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>178</v>
+      <c r="F6" s="29" t="s">
+        <v>175</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>64</v>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>335</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="E7" s="26">
+        <v>174</v>
+      </c>
+      <c r="E7" s="29">
         <v>0</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>178</v>
+      <c r="F7" s="29" t="s">
+        <v>175</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+    </row>
+    <row r="8" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="M8" s="29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="C9" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="B10" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E12" s="29">
         <v>0</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="M8" s="26" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="E9" s="26">
+      <c r="F12" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13" s="32">
         <v>0</v>
       </c>
-      <c r="F9" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E10" s="26">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E11" s="26">
-        <v>0</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="F13" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="M13" s="30" t="s">
         <v>320</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="E12" s="28">
-        <v>0</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2569,38 +2653,35 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
-    </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" style="26" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="26" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.83203125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="26" customWidth="1"/>
-    <col min="8" max="10" width="9.1640625" style="26" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="25" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="13" max="1023" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1024" max="1026" width="9" style="26" customWidth="1"/>
-    <col min="1027" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="19" style="25" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="25" customWidth="1"/>
+    <col min="8" max="10" width="9.1640625" style="25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="13" max="1023" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1024" max="1026" width="9" style="25" customWidth="1"/>
+    <col min="1027" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="70" customHeight="1" x14ac:dyDescent="0.2">
@@ -2611,19 +2692,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -2642,189 +2723,210 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="G3" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="B4" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="G3" s="26" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="26" t="s">
+      <c r="D5" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="C6" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>331</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="C7" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>332</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="C8" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="G8" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8" s="26" t="s">
+      <c r="C9" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C10" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>178</v>
+      <c r="G10" s="25" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>323</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="A11" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="C11" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="L11" s="27"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2843,29 +2945,26 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="11" style="26" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" style="26" customWidth="1"/>
-    <col min="8" max="9" width="9" style="26" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="26" hidden="1"/>
-    <col min="11" max="11" width="15" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="26" customWidth="1"/>
-    <col min="13" max="13" width="9" style="26" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="27.33203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11" style="25" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.1640625" style="25" customWidth="1"/>
+    <col min="8" max="9" width="9" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" style="25" hidden="1"/>
+    <col min="11" max="11" width="15" style="25" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="9" style="25" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -2876,19 +2975,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -2908,21 +3007,21 @@
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>220</v>
+        <v>336</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>64</v>
+        <v>335</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="G3" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2942,9 +3041,6 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2960,7 +3056,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2971,13 +3067,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>44</v>
@@ -2997,22 +3093,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3032,9 +3128,6 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3045,17 +3138,17 @@
     <col min="5" max="5" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.83203125" style="8" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="26" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="26"/>
+    <col min="8" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="12" max="1026" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1027" max="1029" width="9" style="25" customWidth="1"/>
+    <col min="1030" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3066,16 +3159,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>44</v>
@@ -3095,45 +3188,45 @@
     </row>
     <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>123</v>
+        <v>217</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>120</v>
       </c>
       <c r="E3" s="10">
         <v>-3</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>125</v>
+        <v>217</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>122</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3146,25 +3239,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12:F12"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="26" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="26" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="26" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="25" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="25" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" style="6" hidden="1" customWidth="1"/>
     <col min="12" max="1024" width="8.83203125" style="6" customWidth="1"/>
@@ -3172,9 +3262,9 @@
     <col min="1028" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.15">
@@ -3185,16 +3275,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>44</v>
@@ -3213,304 +3303,324 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" s="25">
+        <v>2</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C6" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="25">
+        <v>3</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="D4" s="26">
-        <v>1</v>
-      </c>
-      <c r="E4" s="26">
+      <c r="C7" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25">
         <v>0</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="26" t="s">
+      <c r="F7" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D5" s="26">
-        <v>2</v>
-      </c>
-      <c r="E5" s="26">
+      <c r="C8" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="25">
         <v>0</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D6" s="26">
-        <v>3</v>
-      </c>
-      <c r="E6" s="26">
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="25">
+        <v>6</v>
+      </c>
+      <c r="E9" s="25">
         <v>0</v>
       </c>
-      <c r="F6" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="J6" s="26"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D7" s="26">
-        <v>4</v>
-      </c>
-      <c r="E7" s="26">
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="25">
+        <v>7</v>
+      </c>
+      <c r="E10" s="25">
         <v>0</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="J7" s="26"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="26" t="s">
-        <v>243</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D8" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="26">
-        <v>0</v>
-      </c>
-      <c r="F8" s="26" t="s">
+      <c r="F10" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="J8" s="26"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="26">
-        <v>6</v>
-      </c>
-      <c r="E9" s="26">
-        <v>0</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="J9" s="26"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D10" s="26">
-        <v>7</v>
-      </c>
-      <c r="E10" s="26">
-        <v>0</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>238</v>
+      <c r="C11" s="25" t="s">
+        <v>234</v>
       </c>
       <c r="D11" s="7">
         <v>10000000000</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="25">
         <v>0</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" s="26"/>
+      <c r="F11" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D12" s="26">
+      <c r="A12" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="25">
         <v>3</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="25">
         <v>0</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="26"/>
+      <c r="F12" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="A13" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="25">
         <v>10</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="25">
         <v>0</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="J13" s="26"/>
+      <c r="F13" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26" t="s">
-        <v>252</v>
+      <c r="A14" s="25" t="s">
+        <v>248</v>
       </c>
       <c r="D14" s="7">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="25">
         <v>0</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>253</v>
+      <c r="F14" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="26">
+      <c r="A15" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="25">
         <v>1100</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="25">
         <v>0</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="J15" s="26"/>
+      <c r="F15" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="36">
+      <c r="D16" s="31">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="29" t="s">
-        <v>90</v>
+      <c r="F16" s="28" t="s">
+        <v>87</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D17" s="32">
+        <v>10</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="32" t="s">
+        <v>351</v>
+      </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D18" s="32">
+        <v>1100</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3534,28 +3644,25 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="26" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="26" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="26" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="26" customWidth="1"/>
-    <col min="10" max="1024" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="20" style="25" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="25" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="25" customWidth="1"/>
+    <col min="10" max="1024" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -3566,10 +3673,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>44</v>
@@ -3588,80 +3695,80 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="D5" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="D6" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C7" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="C8" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>264</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>328</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>90</v>
+      <c r="C9" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="H9" s="7"/>
     </row>
@@ -3682,40 +3789,39 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="26"/>
+    <col min="1" max="3" width="9" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G2" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="H2" s="35"/>
+      <c r="I2" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="Q2" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="R2" s="35"/>
+      <c r="S2" s="39" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="34" t="s">
-        <v>267</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="Q2" s="35" t="s">
-        <v>268</v>
-      </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="35" t="s">
-        <v>269</v>
-      </c>
-      <c r="T2" s="31"/>
+      <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -3725,22 +3831,22 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>57</v>
@@ -3749,22 +3855,22 @@
         <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>276</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>31</v>
@@ -3808,15 +3914,14 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1026" max="1028" width="9" style="26" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="8.83203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="75.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1026" max="1028" width="9" style="25" customWidth="1"/>
+    <col min="1029" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -3828,7 +3933,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3836,7 +3941,7 @@
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3844,7 +3949,7 @@
       <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3852,7 +3957,7 @@
       <c r="A5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3860,7 +3965,7 @@
       <c r="A6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3868,7 +3973,7 @@
       <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3876,7 +3981,7 @@
       <c r="A8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3884,7 +3989,7 @@
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3928,19 +4033,18 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="26" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" style="26" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="14" style="25" customWidth="1"/>
+    <col min="2" max="3" width="13.33203125" style="25" customWidth="1"/>
+    <col min="4" max="6" width="9.1640625" style="25" customWidth="1"/>
     <col min="7" max="1017" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3951,7 +4055,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -3991,26 +4095,25 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="26" customWidth="1"/>
-    <col min="3" max="14" width="9.1640625" style="26" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="25" customWidth="1"/>
+    <col min="3" max="14" width="9.1640625" style="25" customWidth="1"/>
     <col min="15" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="H2" s="31"/>
+      <c r="G2" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4020,16 +4123,16 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>31</v>
@@ -4050,10 +4153,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4112,7 +4215,6 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4124,7 +4226,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4135,46 +4237,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="P2" s="18" t="s">
         <v>292</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>296</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>44</v>
@@ -4201,17 +4303,16 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="26"/>
+    <col min="1" max="3" width="9" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4222,28 +4323,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>300</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>304</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4267,17 +4368,16 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="9" style="26" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="26"/>
+    <col min="1" max="3" width="9" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -4288,28 +4388,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>306</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>308</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>309</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>312</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4327,10 +4427,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -4347,15 +4447,14 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="34" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1026" max="1028" width="9" style="26" customWidth="1"/>
-    <col min="1029" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="8.83203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="34" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1026" max="1028" width="9" style="25" customWidth="1"/>
+    <col min="1029" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -4367,7 +4466,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4375,7 +4474,7 @@
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4383,7 +4482,7 @@
       <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4396,7 +4495,7 @@
       <c r="A6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4420,12 +4519,11 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="26" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="25" customWidth="1"/>
     <col min="3" max="1015" width="8.83203125" style="12" customWidth="1"/>
     <col min="1016" max="1018" width="9" style="12" customWidth="1"/>
     <col min="1019" max="16384" width="9" style="12"/>
@@ -4440,7 +4538,7 @@
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4453,7 +4551,7 @@
       <c r="A4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>37</v>
       </c>
     </row>
@@ -4461,7 +4559,7 @@
       <c r="A5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4494,14 +4592,13 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15" style="13" customWidth="1"/>
-    <col min="2" max="2" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="13" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" style="13" customWidth="1"/>
     <col min="4" max="6" width="8.83203125" style="13" customWidth="1"/>
     <col min="7" max="7" width="39.1640625" style="13" customWidth="1"/>
@@ -4541,23 +4638,28 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>66</v>
       </c>
       <c r="D3" s="11"/>
       <c r="G3" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="26"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>334</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4567,39 +4669,38 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMP4"/>
+  <dimension ref="A1:AMP5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
-    </sheetView>
-    <sheetView topLeftCell="F1" workbookViewId="1">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="26" customWidth="1"/>
-    <col min="2" max="3" width="16.1640625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="16" style="26" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="8" style="26" customWidth="1"/>
-    <col min="8" max="16" width="8.83203125" style="26" customWidth="1"/>
-    <col min="17" max="18" width="8.83203125" style="26" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="26" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="1033" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1034" max="1036" width="9" style="26" customWidth="1"/>
-    <col min="1037" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="7.33203125" style="25" customWidth="1"/>
+    <col min="2" max="3" width="16.1640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8" style="25" customWidth="1"/>
+    <col min="8" max="11" width="8.83203125" style="25" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" style="25" customWidth="1"/>
+    <col min="13" max="16" width="8.83203125" style="25" customWidth="1"/>
+    <col min="17" max="18" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="25" customWidth="1"/>
+    <col min="20" max="20" width="11.1640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="1033" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1034" max="1036" width="9" style="25" customWidth="1"/>
+    <col min="1037" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1030" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4610,19 +4711,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="H2" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
+      <c r="M2" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -5646,46 +5747,46 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="J3" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="L3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="M3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="Q3" s="18" t="s">
         <v>44</v>
@@ -6713,50 +6814,98 @@
       <c r="AMP3" s="15"/>
     </row>
     <row r="4" spans="1:1030" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="H4" s="25" t="s">
         <v>84</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>87</v>
       </c>
       <c r="I4" s="7">
         <v>2E-3</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>0</v>
       </c>
-      <c r="K4" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" s="26" t="s">
+      <c r="K4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="25">
+        <v>7.75</v>
+      </c>
+      <c r="O4" s="25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="P4" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="N4" s="26">
+    </row>
+    <row r="5" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2E-3</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="32">
         <v>7.75</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O5" s="32">
         <v>0.77500000000000002</v>
       </c>
-      <c r="P4" s="26" t="s">
-        <v>90</v>
+      <c r="P5" s="32" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -6781,40 +6930,39 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="26" customWidth="1"/>
-    <col min="2" max="2" width="15" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="26" customWidth="1"/>
-    <col min="8" max="8" width="7" style="26" customWidth="1"/>
-    <col min="9" max="9" width="14" style="26" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="26" customWidth="1"/>
-    <col min="11" max="12" width="8.6640625" style="26" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="26" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="26" customWidth="1"/>
-    <col min="15" max="1028" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1029" max="1031" width="9" style="26" customWidth="1"/>
-    <col min="1032" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="9" style="25" customWidth="1"/>
+    <col min="2" max="2" width="15" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="25" customWidth="1"/>
+    <col min="8" max="8" width="7" style="25" customWidth="1"/>
+    <col min="9" max="9" width="14" style="25" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="25" customWidth="1"/>
+    <col min="11" max="12" width="8.6640625" style="25" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="25" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="25" customWidth="1"/>
+    <col min="15" max="1028" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1029" max="1031" width="9" style="25" customWidth="1"/>
+    <col min="1032" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="C2" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -6824,25 +6972,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>99</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>44</v>
@@ -6861,110 +7009,110 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="25">
+        <v>1</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="26">
-        <v>1</v>
-      </c>
-      <c r="H4" s="26">
+      <c r="G5" s="25">
+        <v>2</v>
+      </c>
+      <c r="H5" s="25">
         <v>0</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I5" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="22"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="G6" s="25">
+        <v>3</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="26">
-        <v>2</v>
-      </c>
-      <c r="H5" s="26">
+      <c r="B7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="25">
+        <v>4</v>
+      </c>
+      <c r="H7" s="25">
         <v>0</v>
       </c>
-      <c r="I5" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="I7" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="22"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="26">
-        <v>3</v>
-      </c>
-      <c r="H6" s="26">
+      <c r="B8" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="25">
+        <v>5</v>
+      </c>
+      <c r="H8" s="25">
         <v>0</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="26" t="s">
+      <c r="I8" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="26">
-        <v>4</v>
-      </c>
-      <c r="H7" s="26">
+      <c r="B9" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="25">
+        <v>6</v>
+      </c>
+      <c r="H9" s="25">
         <v>0</v>
       </c>
-      <c r="I7" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="26">
-        <v>5</v>
-      </c>
-      <c r="H8" s="26">
-        <v>0</v>
-      </c>
-      <c r="I8" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="22"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="26">
-        <v>6</v>
-      </c>
-      <c r="H9" s="26">
-        <v>0</v>
-      </c>
-      <c r="I9" s="26" t="s">
-        <v>102</v>
+      <c r="I9" s="25" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -6979,39 +7127,36 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3:I8"/>
-    </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" style="26" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="26" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="26" hidden="1" customWidth="1"/>
-    <col min="11" max="1024" width="9.1640625" style="26" customWidth="1"/>
-    <col min="1025" max="1027" width="9" style="26" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="18" style="25" customWidth="1"/>
+    <col min="2" max="2" width="18" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="25" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="25" hidden="1" customWidth="1"/>
+    <col min="11" max="1024" width="9.1640625" style="25" customWidth="1"/>
+    <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
+    <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -7022,13 +7167,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>44</v>
@@ -7047,118 +7192,152 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="26" t="s">
+      <c r="D4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C5" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="C6" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="C7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="C8" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -7172,40 +7351,37 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
-    </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" style="26" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="19" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="26" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="8.6640625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="26" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="26" customWidth="1"/>
-    <col min="13" max="1026" width="8.83203125" style="26" customWidth="1"/>
-    <col min="1027" max="1029" width="9" style="26" customWidth="1"/>
-    <col min="1030" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="27" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="19" style="25" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="25" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="8.6640625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="25" customWidth="1"/>
+    <col min="13" max="1026" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1027" max="1029" width="9" style="25" customWidth="1"/>
+    <col min="1030" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -7216,19 +7392,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>44</v>
@@ -7247,123 +7423,163 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>87</v>
+      <c r="A3" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E3" s="22">
         <v>1000000000</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>0</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>87</v>
+      <c r="A4" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E4" s="22">
         <v>2000000000</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>0</v>
       </c>
       <c r="G4" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>87</v>
+      <c r="D5" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E5" s="22">
         <v>3000000000</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>0</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>87</v>
+      <c r="A6" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E6" s="22">
         <v>4.0000000000000001E-13</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>0</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>87</v>
+      <c r="A7" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E7" s="22">
         <v>4.9999999999999999E-13</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>0</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>87</v>
+      <c r="A8" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="E8" s="22">
         <v>5.9999999999999997E-13</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>0</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="22">
+        <v>1000000000</v>
+      </c>
+      <c r="F9" s="32">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="22">
+        <v>2000000000</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduce species populations in test_dependencies.xlsx so that discrete/stochastic submodels make significant changes in their populations; ensure that rates of ODE reactions are large enough to make appreciable changes in populations
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -9,7 +9,9 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="460" windowWidth="29800" windowHeight="15300" tabRatio="993" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="-37240" yWindow="1520" windowWidth="20100" windowHeight="10220" tabRatio="993" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="-19620" yWindow="720" windowWidth="18960" windowHeight="11400" tabRatio="500" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="540" yWindow="1340" windowWidth="20040" windowHeight="12900" tabRatio="500" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -83,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="357">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -1066,9 +1068,6 @@
     <t>factor to slow down overly fast reactions</t>
   </si>
   <si>
-    <t>scaling_factor * k_cat_3 * species_1[comp]</t>
-  </si>
-  <si>
     <t>scaling_factor * k_cat_4 * observable_4</t>
   </si>
   <si>
@@ -1139,6 +1138,24 @@
   </si>
   <si>
     <t>density_comp_2</t>
+  </si>
+  <si>
+    <t>rate_law_3_factor</t>
+  </si>
+  <si>
+    <t>factor to speed up rate law 3 so that ODE predications make measureable changes in populations</t>
+  </si>
+  <si>
+    <t>rate_law_8_factor</t>
+  </si>
+  <si>
+    <t>factor to speed up rate law 8 so that ODE predications make measureable changes in populations</t>
+  </si>
+  <si>
+    <t>rate_law_3_factor * scaling_factor * k_cat_3 * species_1[comp]</t>
+  </si>
+  <si>
+    <t>rate_law_8_factor * k_cat_10 * volume_comp</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1272,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1353,6 +1370,9 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1370,6 +1390,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1717,6 +1743,8 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1994,6 +2022,8 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2141,6 +2171,8 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2318,13 +2350,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2358,11 +2394,11 @@
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -2421,7 +2457,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>174</v>
@@ -2442,7 +2478,7 @@
         <v>177</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>309</v>
@@ -2465,7 +2501,7 @@
         <v>179</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>310</v>
@@ -2489,7 +2525,7 @@
         <v>181</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>174</v>
@@ -2513,7 +2549,7 @@
         <v>183</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>313</v>
@@ -2538,7 +2574,7 @@
         <v>185</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>311</v>
@@ -2560,7 +2596,7 @@
         <v>187</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>174</v>
@@ -2582,7 +2618,7 @@
         <v>189</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>174</v>
@@ -2604,7 +2640,7 @@
         <v>316</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>317</v>
@@ -2620,16 +2656,16 @@
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="C13" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>346</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>347</v>
       </c>
       <c r="E13" s="32">
         <v>0</v>
@@ -2660,8 +2696,12 @@
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A5" sqref="A5:XFD10"/>
+    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2762,125 +2802,131 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="41" t="s">
+        <v>355</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="42"/>
+    </row>
+    <row r="6" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G6" s="41" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="K6" s="42"/>
+    </row>
+    <row r="7" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F7" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" s="42"/>
+    </row>
+    <row r="8" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" s="42"/>
+    </row>
+    <row r="9" spans="1:12" s="41" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="41" t="s">
         <v>328</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G9" s="41" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="25" t="s">
+      <c r="K9" s="42"/>
+    </row>
+    <row r="10" spans="1:12" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="G7" s="25" t="s">
+      <c r="F10" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="G10" s="41" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>175</v>
-      </c>
+      <c r="K10" s="42"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
@@ -2909,20 +2955,20 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>348</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>349</v>
-      </c>
       <c r="C12" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>195</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>175</v>
@@ -2945,6 +2991,8 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3007,10 +3055,10 @@
     </row>
     <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>217</v>
@@ -3041,6 +3089,8 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3099,7 +3149,7 @@
         <v>220</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>175</v>
@@ -3128,6 +3178,8 @@
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3239,12 +3291,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="D18" sqref="D18:F18"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3544,9 +3600,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32" t="s">
@@ -3562,9 +3618,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3578,49 +3634,75 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>351</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="D19" s="6">
+        <v>15000</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>353</v>
+      </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D20" s="6">
+        <v>250</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3644,6 +3726,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3789,6 +3873,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3802,26 +3888,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="38" t="s">
+      <c r="H2" s="36"/>
+      <c r="I2" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="Q2" s="39" t="s">
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="Q2" s="40" t="s">
         <v>264</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="39" t="s">
+      <c r="R2" s="36"/>
+      <c r="S2" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="T2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -3914,6 +4000,8 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4033,6 +4121,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4095,6 +4185,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4110,10 +4202,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="40" t="s">
         <v>276</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -4215,6 +4307,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4303,6 +4397,8 @@
       <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4368,6 +4464,8 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4447,6 +4545,8 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4519,6 +4619,8 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4592,8 +4694,10 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4640,25 +4744,25 @@
     </row>
     <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11"/>
       <c r="G3" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="G4" s="13" t="s">
         <v>333</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -4678,6 +4782,8 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4711,19 +4817,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -6862,10 +6968,10 @@
     </row>
     <row r="5" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>337</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>338</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>80</v>
@@ -6893,7 +6999,7 @@
         <v>85</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>84</v>
@@ -6930,6 +7036,8 @@
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6955,14 +7063,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -7134,8 +7242,10 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:A10"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7307,16 +7417,16 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>115</v>
@@ -7324,16 +7434,16 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>108</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>115</v>
@@ -7358,8 +7468,10 @@
       <selection activeCell="Q21" sqref="Q21"/>
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
       <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9:G10"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3:K10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7432,8 +7544,8 @@
       <c r="D3" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="22">
-        <v>1000000000</v>
+      <c r="E3" s="25">
+        <v>1000</v>
       </c>
       <c r="F3" s="25">
         <v>0</v>
@@ -7441,6 +7553,7 @@
       <c r="G3" s="22" t="s">
         <v>115</v>
       </c>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
@@ -7452,8 +7565,8 @@
       <c r="D4" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="22">
-        <v>2000000000</v>
+      <c r="E4" s="25">
+        <v>2000</v>
       </c>
       <c r="F4" s="25">
         <v>0</v>
@@ -7461,6 +7574,7 @@
       <c r="G4" s="22" t="s">
         <v>115</v>
       </c>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
@@ -7472,8 +7586,8 @@
       <c r="D5" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="22">
-        <v>3000000000</v>
+      <c r="E5" s="25">
+        <v>3000</v>
       </c>
       <c r="F5" s="25">
         <v>0</v>
@@ -7481,6 +7595,7 @@
       <c r="G5" s="22" t="s">
         <v>115</v>
       </c>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -7492,8 +7607,8 @@
       <c r="D6" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="22">
-        <v>4.0000000000000001E-13</v>
+      <c r="E6" s="25">
+        <v>3.9999999999999999E-19</v>
       </c>
       <c r="F6" s="25">
         <v>0</v>
@@ -7501,6 +7616,7 @@
       <c r="G6" s="22" t="s">
         <v>132</v>
       </c>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -7512,8 +7628,8 @@
       <c r="D7" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="22">
-        <v>4.9999999999999999E-13</v>
+      <c r="E7" s="25">
+        <v>5.0000000000000004E-19</v>
       </c>
       <c r="F7" s="25">
         <v>0</v>
@@ -7521,6 +7637,7 @@
       <c r="G7" s="22" t="s">
         <v>132</v>
       </c>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
@@ -7532,8 +7649,8 @@
       <c r="D8" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="22">
-        <v>5.9999999999999997E-13</v>
+      <c r="E8" s="25">
+        <v>5.9999999999999999E-19</v>
       </c>
       <c r="F8" s="25">
         <v>0</v>
@@ -7541,19 +7658,20 @@
       <c r="G8" s="22" t="s">
         <v>132</v>
       </c>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="22">
-        <v>1000000000</v>
+      <c r="E9" s="25">
+        <v>1000</v>
       </c>
       <c r="F9" s="32">
         <v>0</v>
@@ -7561,19 +7679,20 @@
       <c r="G9" s="22" t="s">
         <v>115</v>
       </c>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="22">
-        <v>2000000000</v>
+      <c r="E10" s="25">
+        <v>2000</v>
       </c>
       <c r="F10" s="32">
         <v>0</v>
@@ -7581,6 +7700,7 @@
       <c r="G10" s="22" t="s">
         <v>115</v>
       </c>
+      <c r="K10" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
scale up obtain_dependencies() to the H1 WC model currently being created by Yin Hoon; replace the Breadth First Search traversal of the dependency graph with a Depth First Search, using lists of dependencies instead of sets, and using expression and reaction references rather than (class name, expressions instance id) tuples; the improved obtain_dependencies() runs in 10 GB RAM and takes ~70 min on a model with ~21K species, 31K reactions and 29K rate laws
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -9,9 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37240" yWindow="1520" windowWidth="20100" windowHeight="10220" tabRatio="993" firstSheet="3" activeTab="11"/>
-    <workbookView xWindow="-19620" yWindow="720" windowWidth="18960" windowHeight="11400" tabRatio="500" firstSheet="9" activeTab="12"/>
-    <workbookView xWindow="540" yWindow="1340" windowWidth="20040" windowHeight="12900" tabRatio="500" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="1500" yWindow="620" windowWidth="27380" windowHeight="9220" tabRatio="993" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="980" yWindow="10120" windowWidth="28980" windowHeight="11300" tabRatio="500" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -1744,7 +1743,6 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2023,7 +2021,6 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2172,7 +2169,6 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3:C4"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2350,17 +2346,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
       <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2691,17 +2684,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
-      <selection activeCell="A5" sqref="A5:XFD10"/>
-    </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2724,7 +2714,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2992,7 +2982,6 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3090,7 +3079,6 @@
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3179,7 +3167,6 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3299,9 +3286,6 @@
       <selection pane="bottomRight" activeCell="D18" sqref="D18:F18"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3727,7 +3711,6 @@
       <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3874,7 +3857,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4001,7 +3983,6 @@
       <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4122,7 +4103,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4186,7 +4166,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4308,7 +4287,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4398,7 +4376,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4465,7 +4442,6 @@
       <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4546,7 +4522,6 @@
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4620,7 +4595,6 @@
       <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4697,7 +4671,6 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4783,7 +4756,6 @@
       <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7037,7 +7009,6 @@
       <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7245,7 +7216,6 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7471,7 +7441,6 @@
       <selection pane="bottomRight" activeCell="K3" sqref="K3:K10"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Correct the units for dfba_obj_species in fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dependencies.xlsx
+++ b/tests/fixtures/test_dependencies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\karrlab\wc_sim\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="620" windowWidth="27380" windowHeight="9220" tabRatio="993" firstSheet="3" activeTab="12"/>
-    <workbookView xWindow="980" yWindow="10120" windowWidth="28980" windowHeight="11300" tabRatio="500" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="1500" yWindow="615" windowWidth="27375" windowHeight="9225" tabRatio="993" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="975" yWindow="10125" windowWidth="28980" windowHeight="11295" tabRatio="500" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,10 @@
     <definedName name="volume_comp">'!!Functions'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -764,9 +765,6 @@
     <t>biomass_comp_1</t>
   </si>
   <si>
-    <t>M second^-1</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -1155,12 +1153,15 @@
   </si>
   <si>
     <t>rate_law_8_factor * k_cat_10 * volume_comp</t>
+  </si>
+  <si>
+    <t>mole / gDCW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
@@ -1372,6 +1373,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1390,12 +1397,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -1408,6 +1409,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1744,24 +1748,24 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.6640625" style="19" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" style="19" customWidth="1"/>
     <col min="4" max="6" width="9" style="19" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="19" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
@@ -1772,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
@@ -1799,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
@@ -1817,7 +1821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -1826,7 +1830,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>11</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
@@ -1844,7 +1848,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>15</v>
       </c>
@@ -1871,7 +1875,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
@@ -1889,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
@@ -1898,7 +1902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>19</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>20</v>
       </c>
@@ -1916,7 +1920,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>21</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>22</v>
       </c>
@@ -1934,7 +1938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>23</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>24</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>25</v>
       </c>
@@ -1961,7 +1965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>26</v>
       </c>
@@ -1970,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>27</v>
       </c>
@@ -2022,27 +2026,27 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="17" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="17" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="1024" width="8.83203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="17" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="1024" width="8.85546875" style="17" customWidth="1"/>
     <col min="1025" max="1027" width="9" style="17" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -2071,7 +2075,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>137</v>
       </c>
@@ -2083,7 +2087,7 @@
       </c>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>138</v>
       </c>
@@ -2095,7 +2099,7 @@
       </c>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>139</v>
       </c>
@@ -2107,7 +2111,7 @@
       </c>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>140</v>
       </c>
@@ -2118,7 +2122,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>141</v>
       </c>
@@ -2129,7 +2133,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>143</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>145</v>
       </c>
@@ -2170,29 +2174,29 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="25" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="25" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="25" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="25" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.83203125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.85546875" style="25" customWidth="1"/>
     <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2223,7 +2227,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>148</v>
       </c>
@@ -2234,7 +2238,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>149</v>
       </c>
@@ -2245,7 +2249,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>151</v>
       </c>
@@ -2256,7 +2260,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>153</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>155</v>
       </c>
@@ -2278,7 +2282,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>156</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>158</v>
       </c>
@@ -2303,18 +2307,18 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>159</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>160</v>
       </c>
@@ -2325,7 +2329,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>162</v>
       </c>
@@ -2355,50 +2359,50 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="25" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="14" style="25" customWidth="1"/>
-    <col min="4" max="4" width="71.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="25" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="14" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="6.5" style="25" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="25" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="25" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="14" customWidth="1"/>
     <col min="12" max="12" width="5" style="14" customWidth="1"/>
-    <col min="13" max="13" width="37.33203125" style="14" customWidth="1"/>
-    <col min="14" max="1027" width="8.83203125" style="14" customWidth="1"/>
+    <col min="13" max="13" width="37.28515625" style="14" customWidth="1"/>
+    <col min="14" max="1027" width="8.85546875" style="14" customWidth="1"/>
     <col min="1028" max="1030" width="9" style="14" customWidth="1"/>
     <col min="1031" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
     </row>
-    <row r="3" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2446,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>172</v>
       </c>
@@ -2450,7 +2454,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>174</v>
@@ -2463,7 +2467,7 @@
       </c>
       <c r="J4" s="33"/>
     </row>
-    <row r="5" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>176</v>
       </c>
@@ -2471,10 +2475,10 @@
         <v>177</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E5" s="29">
         <v>0</v>
@@ -2486,7 +2490,7 @@
       <c r="H5" s="29"/>
       <c r="J5" s="33"/>
     </row>
-    <row r="6" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>178</v>
       </c>
@@ -2494,10 +2498,10 @@
         <v>179</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E6" s="30">
         <v>0</v>
@@ -2510,7 +2514,7 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
     </row>
-    <row r="7" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>180</v>
       </c>
@@ -2518,7 +2522,7 @@
         <v>181</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>174</v>
@@ -2534,7 +2538,7 @@
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" spans="1:14" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>182</v>
       </c>
@@ -2542,10 +2546,10 @@
         <v>183</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E8" s="29">
         <v>0</v>
@@ -2556,10 +2560,10 @@
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
       <c r="M8" s="29" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>184</v>
       </c>
@@ -2567,10 +2571,10 @@
         <v>185</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="29">
         <v>0</v>
@@ -2581,7 +2585,7 @@
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>186</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>187</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>174</v>
@@ -2603,7 +2607,7 @@
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
     </row>
-    <row r="11" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>188</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>189</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>174</v>
@@ -2625,18 +2629,18 @@
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
     </row>
-    <row r="12" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="C12" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>316</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>334</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>317</v>
       </c>
       <c r="E12" s="29">
         <v>0</v>
@@ -2647,18 +2651,18 @@
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="C13" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>345</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>346</v>
       </c>
       <c r="E13" s="32">
         <v>0</v>
@@ -2667,7 +2671,7 @@
         <v>175</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
@@ -2693,28 +2697,28 @@
     </sheetView>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="25" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="25" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="43.83203125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="25" customWidth="1"/>
-    <col min="8" max="10" width="9.1640625" style="25" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="13" max="1023" width="8.83203125" style="25" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="25" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="25" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="13" max="1023" width="8.85546875" style="25" customWidth="1"/>
     <col min="1024" max="1026" width="9" style="25" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>193</v>
       </c>
@@ -2772,7 +2776,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>197</v>
       </c>
@@ -2792,141 +2796,141 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:12" s="35" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6" spans="1:12" s="35" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="1:12" s="35" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" s="35" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="1:12" s="35" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="1:12" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G10" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="42"/>
-    </row>
-    <row r="6" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>327</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K6" s="42"/>
-    </row>
-    <row r="7" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>329</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K7" s="42"/>
-    </row>
-    <row r="8" spans="1:12" s="41" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>208</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K8" s="42"/>
-    </row>
-    <row r="9" spans="1:12" s="41" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>210</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>328</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K9" s="42"/>
-    </row>
-    <row r="10" spans="1:12" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>319</v>
-      </c>
       <c r="C11" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>195</v>
@@ -2943,22 +2947,22 @@
       <c r="J11" s="27"/>
       <c r="L11" s="27"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>347</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>348</v>
-      </c>
       <c r="C12" s="32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>195</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>175</v>
@@ -2983,28 +2987,28 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="25" customWidth="1"/>
     <col min="2" max="2" width="11" style="25" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" style="25" customWidth="1"/>
     <col min="8" max="9" width="9" style="25" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" style="25" hidden="1"/>
     <col min="11" max="11" width="15" style="25" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="25" customWidth="1"/>
     <col min="13" max="13" width="9" style="25" customWidth="1"/>
     <col min="14" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3042,12 +3046,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>217</v>
@@ -3080,24 +3084,24 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="11" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="11" customWidth="1"/>
     <col min="4" max="4" width="12" style="11" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="1026" width="8.83203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="1026" width="8.85546875" style="12" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="12" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3129,7 +3133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>217</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>220</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>175</v>
@@ -3159,38 +3163,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M17" sqref="M17"/>
       <selection pane="topRight" activeCell="M17" sqref="M17"/>
       <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.1640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="8" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="12" max="1026" width="8.83203125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="8" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="12" max="1026" width="8.85546875" style="25" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="25" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>29</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>224</v>
       </c>
@@ -3242,18 +3246,18 @@
         <v>-3</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="J3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>217</v>
@@ -3265,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>226</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3287,27 +3291,27 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="25" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="25" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="1024" width="8.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="25" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="25" customWidth="1"/>
+    <col min="7" max="9" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="1024" width="8.85546875" style="6" customWidth="1"/>
     <col min="1025" max="1027" width="9" style="6" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>90</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F2" s="18" t="s">
         <v>76</v>
@@ -3342,12 +3346,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>233</v>
       </c>
       <c r="D3" s="25">
         <v>0.3</v>
@@ -3357,12 +3361,12 @@
       </c>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>196</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D4" s="25">
         <v>1</v>
@@ -3375,12 +3379,12 @@
       </c>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" s="25">
         <v>2</v>
@@ -3393,12 +3397,12 @@
       </c>
       <c r="J5" s="25"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="25">
         <v>3</v>
@@ -3407,16 +3411,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="25" t="s">
-        <v>238</v>
-      </c>
       <c r="C7" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" s="25">
         <v>4</v>
@@ -3425,16 +3429,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J7" s="25"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D8" s="25">
         <v>0.5</v>
@@ -3443,16 +3447,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="J8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="25" t="s">
-        <v>241</v>
-      </c>
       <c r="C9" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D9" s="25">
         <v>6</v>
@@ -3461,16 +3465,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="J9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="25" t="s">
-        <v>243</v>
-      </c>
       <c r="C10" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D10" s="25">
         <v>7</v>
@@ -3483,12 +3487,12 @@
       </c>
       <c r="J10" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" s="7">
         <v>10000000000</v>
@@ -3501,12 +3505,12 @@
       </c>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D12" s="25">
         <v>3</v>
@@ -3519,12 +3523,12 @@
       </c>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D13" s="25">
         <v>10</v>
@@ -3533,13 +3537,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
         <v>247</v>
-      </c>
-      <c r="J13" s="25"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25" t="s">
-        <v>248</v>
       </c>
       <c r="D14" s="7">
         <v>6.0221407599999999E+23</v>
@@ -3548,11 +3552,11 @@
         <v>0</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>86</v>
       </c>
@@ -3567,9 +3571,9 @@
       </c>
       <c r="J15" s="25"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -3581,16 +3585,16 @@
         <v>87</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="32">
         <v>10</v>
@@ -3602,9 +3606,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -3618,9 +3622,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -3634,12 +3638,12 @@
         <v>87</v>
       </c>
       <c r="J19" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="B20" s="6"/>
       <c r="D20" s="6">
@@ -3655,38 +3659,38 @@
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
       <c r="J20" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3712,27 +3716,27 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="25" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="25" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="25" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="8.83203125" style="25" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="25" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="25" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="25" customWidth="1"/>
-    <col min="10" max="1024" width="8.83203125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="25" customWidth="1"/>
+    <col min="10" max="1024" width="8.85546875" style="25" customWidth="1"/>
     <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -3761,78 +3765,78 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>252</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>253</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>254</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>255</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>256</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>257</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>87</v>
@@ -3849,49 +3853,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M16" sqref="M16"/>
-      <selection pane="topRight" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9" style="25" customWidth="1"/>
     <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="41" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="G2" s="39" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="39" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="Q2" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="Q2" s="40" t="s">
+      <c r="R2" s="38"/>
+      <c r="S2" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="R2" s="36"/>
-      <c r="S2" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="T2" s="36"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T2" s="38"/>
+    </row>
+    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -3902,7 +3900,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>76</v>
@@ -3911,10 +3909,10 @@
         <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>267</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>57</v>
@@ -3926,19 +3924,19 @@
         <v>67</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>272</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>31</v>
@@ -3984,21 +3982,21 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="75.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="25" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.85546875" style="25" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="25" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4006,7 +4004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
@@ -4014,7 +4012,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>33</v>
       </c>
@@ -4022,7 +4020,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>35</v>
       </c>
@@ -4030,7 +4028,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>37</v>
       </c>
@@ -4038,7 +4036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
@@ -4046,7 +4044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>41</v>
       </c>
@@ -4054,7 +4052,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
@@ -4062,22 +4060,22 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>47</v>
       </c>
@@ -4104,20 +4102,20 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="25" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" style="25" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="25" customWidth="1"/>
-    <col min="7" max="1017" width="9.1640625" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" style="25" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="25" customWidth="1"/>
+    <col min="7" max="1017" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -4125,7 +4123,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>44</v>
@@ -4137,13 +4135,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -4158,35 +4156,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="M16" sqref="M16"/>
-      <selection pane="topRight" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
-      <selection pane="bottomRight" activeCell="M16" sqref="M16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="25" customWidth="1"/>
-    <col min="3" max="14" width="9.1640625" style="25" customWidth="1"/>
-    <col min="15" max="1024" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="25" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="25" customWidth="1"/>
+    <col min="15" max="1024" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="42" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>29</v>
       </c>
@@ -4197,7 +4189,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>76</v>
@@ -4224,41 +4216,41 @@
         <v>54</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
@@ -4288,20 +4280,20 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="8.83203125" style="2" customWidth="1"/>
-    <col min="18" max="1025" width="8.83203125" style="3" customWidth="1"/>
+    <col min="1" max="17" width="8.85546875" style="2" customWidth="1"/>
+    <col min="18" max="1025" width="8.85546875" style="3" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="3" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4309,46 +4301,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>282</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>283</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>96</v>
       </c>
       <c r="H2" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="O2" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="P2" s="18" t="s">
         <v>291</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>292</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>44</v>
@@ -4377,18 +4369,18 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9" style="25" customWidth="1"/>
     <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4396,28 +4388,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>299</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>300</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4443,18 +4435,18 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9" style="25" customWidth="1"/>
     <col min="4" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4465,25 +4457,25 @@
         <v>96</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>303</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>307</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>308</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>44</v>
@@ -4501,10 +4493,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -4523,21 +4515,21 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="34" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" style="25" customWidth="1"/>
+    <col min="3" max="1025" width="8.85546875" style="25" customWidth="1"/>
     <col min="1026" max="1028" width="9" style="25" customWidth="1"/>
     <col min="1029" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4545,7 +4537,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
@@ -4553,7 +4545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
@@ -4561,12 +4553,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>45</v>
       </c>
@@ -4574,7 +4566,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>54</v>
       </c>
@@ -4596,21 +4588,21 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="25" customWidth="1"/>
-    <col min="3" max="1015" width="8.83203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="25" customWidth="1"/>
+    <col min="3" max="1015" width="8.85546875" style="12" customWidth="1"/>
     <col min="1016" max="1018" width="9" style="12" customWidth="1"/>
     <col min="1019" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4618,12 +4610,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>57</v>
       </c>
@@ -4631,7 +4623,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>58</v>
       </c>
@@ -4639,17 +4631,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>54</v>
       </c>
@@ -4672,24 +4664,24 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" style="13" customWidth="1"/>
-    <col min="4" max="6" width="8.83203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="39.1640625" style="13" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="13" customWidth="1"/>
+    <col min="4" max="6" width="8.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" style="13" customWidth="1"/>
+    <col min="8" max="1026" width="8.85546875" style="17" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="17" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -4715,27 +4707,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="11"/>
       <c r="G3" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
+      <c r="C4" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="G4" s="13" t="s">
         <v>332</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -4757,31 +4749,31 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="25" customWidth="1"/>
-    <col min="2" max="3" width="16.1640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="25" customWidth="1"/>
+    <col min="2" max="3" width="16.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="25" customWidth="1"/>
     <col min="5" max="5" width="16" style="25" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="25" customWidth="1"/>
     <col min="7" max="7" width="8" style="25" customWidth="1"/>
-    <col min="8" max="11" width="8.83203125" style="25" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" style="25" customWidth="1"/>
-    <col min="13" max="16" width="8.83203125" style="25" customWidth="1"/>
-    <col min="17" max="18" width="8.83203125" style="25" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="25" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="1033" width="8.83203125" style="25" customWidth="1"/>
+    <col min="8" max="11" width="8.85546875" style="25" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="25" customWidth="1"/>
+    <col min="13" max="16" width="8.85546875" style="25" customWidth="1"/>
+    <col min="17" max="18" width="8.85546875" style="25" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="25" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="1033" width="8.85546875" style="25" customWidth="1"/>
     <col min="1034" max="1036" width="9" style="25" customWidth="1"/>
     <col min="1037" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1030" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1030" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -4789,19 +4781,19 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -5817,7 +5809,7 @@
       <c r="AMO2" s="15"/>
       <c r="AMP2" s="15"/>
     </row>
-    <row r="3" spans="1:1030" ht="56" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1030" ht="56.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -6891,7 +6883,7 @@
       <c r="AMO3" s="15"/>
       <c r="AMP3" s="15"/>
     </row>
-    <row r="4" spans="1:1030" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1030" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>78</v>
       </c>
@@ -6938,12 +6930,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1030" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>336</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>337</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>80</v>
@@ -6971,7 +6963,7 @@
         <v>85</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>84</v>
@@ -7001,49 +6993,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="Q21" sqref="Q21"/>
-      <selection pane="topRight" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="25" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="25" customWidth="1"/>
+    <col min="3" max="5" width="8.85546875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="25" customWidth="1"/>
     <col min="8" max="8" width="7" style="25" customWidth="1"/>
     <col min="9" max="9" width="14" style="25" customWidth="1"/>
-    <col min="10" max="10" width="18.5" style="25" customWidth="1"/>
-    <col min="11" max="12" width="8.6640625" style="25" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="25" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="25" customWidth="1"/>
-    <col min="15" max="1028" width="8.83203125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="25" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="25" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" style="25" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="25" customWidth="1"/>
+    <col min="15" max="1028" width="8.85546875" style="25" customWidth="1"/>
     <col min="1029" max="1031" width="9" style="25" customWidth="1"/>
     <col min="1032" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="35" t="s">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -7087,7 +7073,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>97</v>
       </c>
@@ -7105,7 +7091,7 @@
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>100</v>
       </c>
@@ -7123,7 +7109,7 @@
       </c>
       <c r="J5" s="22"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>102</v>
       </c>
@@ -7141,7 +7127,7 @@
       </c>
       <c r="J6" s="22"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
@@ -7159,7 +7145,7 @@
       </c>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>106</v>
       </c>
@@ -7177,7 +7163,7 @@
       </c>
       <c r="J8" s="22"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>108</v>
       </c>
@@ -7217,29 +7203,29 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="25" customWidth="1"/>
     <col min="2" max="2" width="18" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="25" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="25" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="25" hidden="1" customWidth="1"/>
-    <col min="11" max="1024" width="9.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="25" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="25" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="25" hidden="1" customWidth="1"/>
+    <col min="11" max="1024" width="9.140625" style="25" customWidth="1"/>
     <col min="1025" max="1027" width="9" style="25" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -7271,7 +7257,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>113</v>
       </c>
@@ -7290,7 +7276,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>116</v>
       </c>
@@ -7309,7 +7295,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>118</v>
       </c>
@@ -7328,7 +7314,7 @@
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>120</v>
       </c>
@@ -7347,7 +7333,7 @@
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>122</v>
       </c>
@@ -7366,7 +7352,7 @@
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>124</v>
       </c>
@@ -7385,35 +7371,35 @@
       <c r="I8" s="24"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>108</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>115</v>
@@ -7442,30 +7428,30 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="25" customWidth="1"/>
     <col min="3" max="3" width="19" style="25" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="25" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="8.6640625" style="25" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="25" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="25" customWidth="1"/>
-    <col min="13" max="1026" width="8.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="25" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="8.7109375" style="25" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="25" customWidth="1"/>
+    <col min="13" max="1026" width="8.85546875" style="25" customWidth="1"/>
     <col min="1027" max="1029" width="9" style="25" customWidth="1"/>
     <col min="1030" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>29</v>
       </c>
@@ -7503,7 +7489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>128</v>
       </c>
@@ -7524,7 +7510,7 @@
       </c>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>129</v>
       </c>
@@ -7545,7 +7531,7 @@
       </c>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>130</v>
       </c>
@@ -7566,7 +7552,7 @@
       </c>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>131</v>
       </c>
@@ -7587,7 +7573,7 @@
       </c>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>133</v>
       </c>
@@ -7608,7 +7594,7 @@
       </c>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:12" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>134</v>
       </c>
@@ -7629,12 +7615,12 @@
       </c>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>84</v>
@@ -7650,12 +7636,12 @@
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>84</v>

</xml_diff>